<commit_message>
work on plots for publication with dig properties
</commit_message>
<xml_diff>
--- a/data-dig-prop-stats/dat.xlsx
+++ b/data-dig-prop-stats/dat.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28129"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29426"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://aarhusuniversitet-my.sharepoint.com/personal/au583430_uni_au_dk/Documents/Documents/GitHub/Pedersen-2024-MAG/data-dig-prop-stats/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://aarhusuniversitet-my.sharepoint.com/personal/au583430_uni_au_dk/Documents/Documents/GitHub/Pedersen-2025-MAG/data-dig-prop-stats/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="384" documentId="8_{7A56C225-DD08-4D66-98D8-C216CC569554}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{4374CC52-357C-47FA-AD62-151D59C509F0}"/>
+  <xr:revisionPtr revIDLastSave="451" documentId="8_{7A56C225-DD08-4D66-98D8-C216CC569554}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{3798FE73-5FC1-5FDE-9258-5F69D6DB3755}"/>
   <bookViews>
-    <workbookView xWindow="-30225" yWindow="150" windowWidth="26310" windowHeight="20220" activeTab="3" xr2:uid="{C233AD18-B618-41A4-BC30-2DA8BD150481}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17520" xr2:uid="{C233AD18-B618-41A4-BC30-2DA8BD150481}"/>
   </bookViews>
   <sheets>
     <sheet name="slurry" sheetId="1" r:id="rId1"/>
@@ -774,8 +774,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{219A4E69-9D4D-4283-8C99-A6FA113EB291}">
   <dimension ref="A1:V77"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="J17" sqref="J17"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D6" sqref="D6:D8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -6462,8 +6462,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{01BD706F-A0B7-4D5E-B189-117437D2C46D}">
   <dimension ref="A1:G77"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A29" workbookViewId="0">
-      <selection activeCell="M66" sqref="M66"/>
+    <sheetView topLeftCell="A8" workbookViewId="0">
+      <selection activeCell="G49" sqref="G49"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>

</xml_diff>